<commit_message>
notas tabelas, imagens, gráficos
</commit_message>
<xml_diff>
--- a/artigo/tabela_medias_Conforto_Carisma.xlsx
+++ b/artigo/tabela_medias_Conforto_Carisma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.andreotti\Desktop\python_Inegradora_II\artigo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.andreotti\Desktop\03 - Integradora\python_Inegradora_II\artigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AE2C3C-A0A7-4EF3-8237-9D11F87CC117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12429F53-6D73-4266-A3E7-02CFFA784938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25A7948E-7D82-4246-8204-219A589AA784}"/>
+    <workbookView xWindow="75" yWindow="120" windowWidth="25965" windowHeight="13695" xr2:uid="{25A7948E-7D82-4246-8204-219A589AA784}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>_SEM_FILTRO</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Conforto</t>
+  </si>
+  <si>
+    <t>Insights</t>
+  </si>
+  <si>
+    <t>ta tudo igual (????????)</t>
+  </si>
+  <si>
+    <t>Os participantes acharam a personagem confortável/normal</t>
+  </si>
+  <si>
+    <t>Os participantes não acharam a personagem desconfortável</t>
   </si>
 </sst>
 </file>
@@ -433,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BE3BB0-968E-4E19-853B-03A8E64876D0}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:I20"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,6 +818,26 @@
         <v>3.1305999999999998</v>
       </c>
     </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>